<commit_message>
fixing bowtie paired end
</commit_message>
<xml_diff>
--- a/WGS/paired end scripts.xlsx
+++ b/WGS/paired end scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.studivan/Documents/GitHub/SCTLD-resistance-genomics/WGS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC44DD92-0B3A-C74F-A8A4-53C467FE1DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066F743A-4A15-A046-8CC0-28669D8C9E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6880" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{ADDD3B2E-9B5B-4147-8B7E-5AA001AF2620}"/>
   </bookViews>
@@ -7110,8 +7110,8 @@
         <v>720</v>
       </c>
       <c r="H1" t="str">
-        <f>"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A1&amp;" -2 "&amp;C1&amp;" -S "&amp;F1&amp;".bt2.sam --no-unal --al ./"&amp;F1&amp;".al --un symbionts/"&amp;F1&amp;".un"</f>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s001_R1_001_val_1.fq.gz -2 s001_R2_001_val_2.fq.gz -S s001.bt2.sam --no-unal --al ./s001.al --un symbionts/s001.un</v>
+        <f>"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A1&amp;" -2 "&amp;C1&amp;" -S "&amp;F1&amp;".bt2.sam --no-unal --al-conc ./"&amp;F1&amp;".al --un-conc symbionts/"&amp;F1&amp;".un"</f>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s001_R1_001_val_1.fq.gz -2 s001_R2_001_val_2.fq.gz -S s001.bt2.sam --no-unal --al-conc ./s001.al --un-conc symbionts/s001.un</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -7125,8 +7125,8 @@
         <v>721</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H65" si="0">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A2&amp;" -2 "&amp;C2&amp;" -S "&amp;F2&amp;".bt2.sam --no-unal --al ./"&amp;F2&amp;".al --un symbionts/"&amp;F2&amp;".un"</f>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s002_R1_001_val_1.fq.gz -2 s002_R2_001_val_2.fq.gz -S s002.bt2.sam --no-unal --al ./s002.al --un symbionts/s002.un</v>
+        <f t="shared" ref="H2:H65" si="0">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A2&amp;" -2 "&amp;C2&amp;" -S "&amp;F2&amp;".bt2.sam --no-unal --al-conc ./"&amp;F2&amp;".al --un-conc symbionts/"&amp;F2&amp;".un"</f>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s002_R1_001_val_1.fq.gz -2 s002_R2_001_val_2.fq.gz -S s002.bt2.sam --no-unal --al-conc ./s002.al --un-conc symbionts/s002.un</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s003_R1_001_val_1.fq.gz -2 s003_R2_001_val_2.fq.gz -S s003.bt2.sam --no-unal --al ./s003.al --un symbionts/s003.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s003_R1_001_val_1.fq.gz -2 s003_R2_001_val_2.fq.gz -S s003.bt2.sam --no-unal --al-conc ./s003.al --un-conc symbionts/s003.un</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -7156,7 +7156,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s004_R1_001_val_1.fq.gz -2 s004_R2_001_val_2.fq.gz -S s004.bt2.sam --no-unal --al ./s004.al --un symbionts/s004.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s004_R1_001_val_1.fq.gz -2 s004_R2_001_val_2.fq.gz -S s004.bt2.sam --no-unal --al-conc ./s004.al --un-conc symbionts/s004.un</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7171,7 +7171,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s005_R1_001_val_1.fq.gz -2 s005_R2_001_val_2.fq.gz -S s005.bt2.sam --no-unal --al ./s005.al --un symbionts/s005.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s005_R1_001_val_1.fq.gz -2 s005_R2_001_val_2.fq.gz -S s005.bt2.sam --no-unal --al-conc ./s005.al --un-conc symbionts/s005.un</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -7186,7 +7186,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s006_R1_001_val_1.fq.gz -2 s006_R2_001_val_2.fq.gz -S s006.bt2.sam --no-unal --al ./s006.al --un symbionts/s006.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s006_R1_001_val_1.fq.gz -2 s006_R2_001_val_2.fq.gz -S s006.bt2.sam --no-unal --al-conc ./s006.al --un-conc symbionts/s006.un</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s007_R1_001_val_1.fq.gz -2 s007_R2_001_val_2.fq.gz -S s007.bt2.sam --no-unal --al ./s007.al --un symbionts/s007.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s007_R1_001_val_1.fq.gz -2 s007_R2_001_val_2.fq.gz -S s007.bt2.sam --no-unal --al-conc ./s007.al --un-conc symbionts/s007.un</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -7216,7 +7216,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s008_R1_001_val_1.fq.gz -2 s008_R2_001_val_2.fq.gz -S s008.bt2.sam --no-unal --al ./s008.al --un symbionts/s008.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s008_R1_001_val_1.fq.gz -2 s008_R2_001_val_2.fq.gz -S s008.bt2.sam --no-unal --al-conc ./s008.al --un-conc symbionts/s008.un</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -7231,7 +7231,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s009_R1_001_val_1.fq.gz -2 s009_R2_001_val_2.fq.gz -S s009.bt2.sam --no-unal --al ./s009.al --un symbionts/s009.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s009_R1_001_val_1.fq.gz -2 s009_R2_001_val_2.fq.gz -S s009.bt2.sam --no-unal --al-conc ./s009.al --un-conc symbionts/s009.un</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s010_R1_001_val_1.fq.gz -2 s010_R2_001_val_2.fq.gz -S s010.bt2.sam --no-unal --al ./s010.al --un symbionts/s010.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s010_R1_001_val_1.fq.gz -2 s010_R2_001_val_2.fq.gz -S s010.bt2.sam --no-unal --al-conc ./s010.al --un-conc symbionts/s010.un</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -7261,7 +7261,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s011_R1_001_val_1.fq.gz -2 s011_R2_001_val_2.fq.gz -S s011.bt2.sam --no-unal --al ./s011.al --un symbionts/s011.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s011_R1_001_val_1.fq.gz -2 s011_R2_001_val_2.fq.gz -S s011.bt2.sam --no-unal --al-conc ./s011.al --un-conc symbionts/s011.un</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -7276,7 +7276,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s012_R1_001_val_1.fq.gz -2 s012_R2_001_val_2.fq.gz -S s012.bt2.sam --no-unal --al ./s012.al --un symbionts/s012.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s012_R1_001_val_1.fq.gz -2 s012_R2_001_val_2.fq.gz -S s012.bt2.sam --no-unal --al-conc ./s012.al --un-conc symbionts/s012.un</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -7291,7 +7291,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s013_R1_001_val_1.fq.gz -2 s013_R2_001_val_2.fq.gz -S s013.bt2.sam --no-unal --al ./s013.al --un symbionts/s013.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s013_R1_001_val_1.fq.gz -2 s013_R2_001_val_2.fq.gz -S s013.bt2.sam --no-unal --al-conc ./s013.al --un-conc symbionts/s013.un</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -7306,7 +7306,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s014_R1_001_val_1.fq.gz -2 s014_R2_001_val_2.fq.gz -S s014.bt2.sam --no-unal --al ./s014.al --un symbionts/s014.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s014_R1_001_val_1.fq.gz -2 s014_R2_001_val_2.fq.gz -S s014.bt2.sam --no-unal --al-conc ./s014.al --un-conc symbionts/s014.un</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -7321,7 +7321,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s015_R1_001_val_1.fq.gz -2 s015_R2_001_val_2.fq.gz -S s015.bt2.sam --no-unal --al ./s015.al --un symbionts/s015.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s015_R1_001_val_1.fq.gz -2 s015_R2_001_val_2.fq.gz -S s015.bt2.sam --no-unal --al-conc ./s015.al --un-conc symbionts/s015.un</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -7336,7 +7336,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s016_R1_001_val_1.fq.gz -2 s016_R2_001_val_2.fq.gz -S s016.bt2.sam --no-unal --al ./s016.al --un symbionts/s016.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s016_R1_001_val_1.fq.gz -2 s016_R2_001_val_2.fq.gz -S s016.bt2.sam --no-unal --al-conc ./s016.al --un-conc symbionts/s016.un</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -7351,7 +7351,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s017_R1_001_val_1.fq.gz -2 s017_R2_001_val_2.fq.gz -S s017.bt2.sam --no-unal --al ./s017.al --un symbionts/s017.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s017_R1_001_val_1.fq.gz -2 s017_R2_001_val_2.fq.gz -S s017.bt2.sam --no-unal --al-conc ./s017.al --un-conc symbionts/s017.un</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s018_R1_001_val_1.fq.gz -2 s018_R2_001_val_2.fq.gz -S s018.bt2.sam --no-unal --al ./s018.al --un symbionts/s018.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s018_R1_001_val_1.fq.gz -2 s018_R2_001_val_2.fq.gz -S s018.bt2.sam --no-unal --al-conc ./s018.al --un-conc symbionts/s018.un</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -7381,7 +7381,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s019_R1_001_val_1.fq.gz -2 s019_R2_001_val_2.fq.gz -S s019.bt2.sam --no-unal --al ./s019.al --un symbionts/s019.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s019_R1_001_val_1.fq.gz -2 s019_R2_001_val_2.fq.gz -S s019.bt2.sam --no-unal --al-conc ./s019.al --un-conc symbionts/s019.un</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -7396,7 +7396,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s020_R1_001_val_1.fq.gz -2 s020_R2_001_val_2.fq.gz -S s020.bt2.sam --no-unal --al ./s020.al --un symbionts/s020.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s020_R1_001_val_1.fq.gz -2 s020_R2_001_val_2.fq.gz -S s020.bt2.sam --no-unal --al-conc ./s020.al --un-conc symbionts/s020.un</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -7411,7 +7411,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s021_R1_001_val_1.fq.gz -2 s021_R2_001_val_2.fq.gz -S s021.bt2.sam --no-unal --al ./s021.al --un symbionts/s021.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s021_R1_001_val_1.fq.gz -2 s021_R2_001_val_2.fq.gz -S s021.bt2.sam --no-unal --al-conc ./s021.al --un-conc symbionts/s021.un</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -7426,7 +7426,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s022_R1_001_val_1.fq.gz -2 s022_R2_001_val_2.fq.gz -S s022.bt2.sam --no-unal --al ./s022.al --un symbionts/s022.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s022_R1_001_val_1.fq.gz -2 s022_R2_001_val_2.fq.gz -S s022.bt2.sam --no-unal --al-conc ./s022.al --un-conc symbionts/s022.un</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s023_R1_001_val_1.fq.gz -2 s023_R2_001_val_2.fq.gz -S s023.bt2.sam --no-unal --al ./s023.al --un symbionts/s023.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s023_R1_001_val_1.fq.gz -2 s023_R2_001_val_2.fq.gz -S s023.bt2.sam --no-unal --al-conc ./s023.al --un-conc symbionts/s023.un</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -7456,7 +7456,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s024_R1_001_val_1.fq.gz -2 s024_R2_001_val_2.fq.gz -S s024.bt2.sam --no-unal --al ./s024.al --un symbionts/s024.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s024_R1_001_val_1.fq.gz -2 s024_R2_001_val_2.fq.gz -S s024.bt2.sam --no-unal --al-conc ./s024.al --un-conc symbionts/s024.un</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s025_R1_001_val_1.fq.gz -2 s025_R2_001_val_2.fq.gz -S s025.bt2.sam --no-unal --al ./s025.al --un symbionts/s025.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s025_R1_001_val_1.fq.gz -2 s025_R2_001_val_2.fq.gz -S s025.bt2.sam --no-unal --al-conc ./s025.al --un-conc symbionts/s025.un</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -7486,7 +7486,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s026_R1_001_val_1.fq.gz -2 s026_R2_001_val_2.fq.gz -S s026.bt2.sam --no-unal --al ./s026.al --un symbionts/s026.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s026_R1_001_val_1.fq.gz -2 s026_R2_001_val_2.fq.gz -S s026.bt2.sam --no-unal --al-conc ./s026.al --un-conc symbionts/s026.un</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -7501,7 +7501,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s027_R1_001_val_1.fq.gz -2 s027_R2_001_val_2.fq.gz -S s027.bt2.sam --no-unal --al ./s027.al --un symbionts/s027.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s027_R1_001_val_1.fq.gz -2 s027_R2_001_val_2.fq.gz -S s027.bt2.sam --no-unal --al-conc ./s027.al --un-conc symbionts/s027.un</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -7516,7 +7516,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s028_R1_001_val_1.fq.gz -2 s028_R2_001_val_2.fq.gz -S s028.bt2.sam --no-unal --al ./s028.al --un symbionts/s028.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s028_R1_001_val_1.fq.gz -2 s028_R2_001_val_2.fq.gz -S s028.bt2.sam --no-unal --al-conc ./s028.al --un-conc symbionts/s028.un</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -7531,7 +7531,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s029_R1_001_val_1.fq.gz -2 s029_R2_001_val_2.fq.gz -S s029.bt2.sam --no-unal --al ./s029.al --un symbionts/s029.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s029_R1_001_val_1.fq.gz -2 s029_R2_001_val_2.fq.gz -S s029.bt2.sam --no-unal --al-conc ./s029.al --un-conc symbionts/s029.un</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -7546,7 +7546,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s030_R1_001_val_1.fq.gz -2 s030_R2_001_val_2.fq.gz -S s030.bt2.sam --no-unal --al ./s030.al --un symbionts/s030.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s030_R1_001_val_1.fq.gz -2 s030_R2_001_val_2.fq.gz -S s030.bt2.sam --no-unal --al-conc ./s030.al --un-conc symbionts/s030.un</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s031_R1_001_val_1.fq.gz -2 s031_R2_001_val_2.fq.gz -S s031.bt2.sam --no-unal --al ./s031.al --un symbionts/s031.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s031_R1_001_val_1.fq.gz -2 s031_R2_001_val_2.fq.gz -S s031.bt2.sam --no-unal --al-conc ./s031.al --un-conc symbionts/s031.un</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -7576,7 +7576,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s032_R1_001_val_1.fq.gz -2 s032_R2_001_val_2.fq.gz -S s032.bt2.sam --no-unal --al ./s032.al --un symbionts/s032.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s032_R1_001_val_1.fq.gz -2 s032_R2_001_val_2.fq.gz -S s032.bt2.sam --no-unal --al-conc ./s032.al --un-conc symbionts/s032.un</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -7591,7 +7591,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s033_R1_001_val_1.fq.gz -2 s033_R2_001_val_2.fq.gz -S s033.bt2.sam --no-unal --al ./s033.al --un symbionts/s033.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s033_R1_001_val_1.fq.gz -2 s033_R2_001_val_2.fq.gz -S s033.bt2.sam --no-unal --al-conc ./s033.al --un-conc symbionts/s033.un</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -7606,7 +7606,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s034_R1_001_val_1.fq.gz -2 s034_R2_001_val_2.fq.gz -S s034.bt2.sam --no-unal --al ./s034.al --un symbionts/s034.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s034_R1_001_val_1.fq.gz -2 s034_R2_001_val_2.fq.gz -S s034.bt2.sam --no-unal --al-conc ./s034.al --un-conc symbionts/s034.un</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s035_R1_001_val_1.fq.gz -2 s035_R2_001_val_2.fq.gz -S s035.bt2.sam --no-unal --al ./s035.al --un symbionts/s035.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s035_R1_001_val_1.fq.gz -2 s035_R2_001_val_2.fq.gz -S s035.bt2.sam --no-unal --al-conc ./s035.al --un-conc symbionts/s035.un</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -7636,7 +7636,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s036_R1_001_val_1.fq.gz -2 s036_R2_001_val_2.fq.gz -S s036.bt2.sam --no-unal --al ./s036.al --un symbionts/s036.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s036_R1_001_val_1.fq.gz -2 s036_R2_001_val_2.fq.gz -S s036.bt2.sam --no-unal --al-conc ./s036.al --un-conc symbionts/s036.un</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -7651,7 +7651,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s037_R1_001_val_1.fq.gz -2 s037_R2_001_val_2.fq.gz -S s037.bt2.sam --no-unal --al ./s037.al --un symbionts/s037.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s037_R1_001_val_1.fq.gz -2 s037_R2_001_val_2.fq.gz -S s037.bt2.sam --no-unal --al-conc ./s037.al --un-conc symbionts/s037.un</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -7666,7 +7666,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s038_R1_001_val_1.fq.gz -2 s038_R2_001_val_2.fq.gz -S s038.bt2.sam --no-unal --al ./s038.al --un symbionts/s038.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s038_R1_001_val_1.fq.gz -2 s038_R2_001_val_2.fq.gz -S s038.bt2.sam --no-unal --al-conc ./s038.al --un-conc symbionts/s038.un</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s039_R1_001_val_1.fq.gz -2 s039_R2_001_val_2.fq.gz -S s039.bt2.sam --no-unal --al ./s039.al --un symbionts/s039.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s039_R1_001_val_1.fq.gz -2 s039_R2_001_val_2.fq.gz -S s039.bt2.sam --no-unal --al-conc ./s039.al --un-conc symbionts/s039.un</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -7696,7 +7696,7 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s040_R1_001_val_1.fq.gz -2 s040_R2_001_val_2.fq.gz -S s040.bt2.sam --no-unal --al ./s040.al --un symbionts/s040.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s040_R1_001_val_1.fq.gz -2 s040_R2_001_val_2.fq.gz -S s040.bt2.sam --no-unal --al-conc ./s040.al --un-conc symbionts/s040.un</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -7711,7 +7711,7 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s041_R1_001_val_1.fq.gz -2 s041_R2_001_val_2.fq.gz -S s041.bt2.sam --no-unal --al ./s041.al --un symbionts/s041.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s041_R1_001_val_1.fq.gz -2 s041_R2_001_val_2.fq.gz -S s041.bt2.sam --no-unal --al-conc ./s041.al --un-conc symbionts/s041.un</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -7726,7 +7726,7 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s042_R1_001_val_1.fq.gz -2 s042_R2_001_val_2.fq.gz -S s042.bt2.sam --no-unal --al ./s042.al --un symbionts/s042.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s042_R1_001_val_1.fq.gz -2 s042_R2_001_val_2.fq.gz -S s042.bt2.sam --no-unal --al-conc ./s042.al --un-conc symbionts/s042.un</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -7741,7 +7741,7 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s043_R1_001_val_1.fq.gz -2 s043_R2_001_val_2.fq.gz -S s043.bt2.sam --no-unal --al ./s043.al --un symbionts/s043.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s043_R1_001_val_1.fq.gz -2 s043_R2_001_val_2.fq.gz -S s043.bt2.sam --no-unal --al-conc ./s043.al --un-conc symbionts/s043.un</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -7756,7 +7756,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s044_R1_001_val_1.fq.gz -2 s044_R2_001_val_2.fq.gz -S s044.bt2.sam --no-unal --al ./s044.al --un symbionts/s044.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s044_R1_001_val_1.fq.gz -2 s044_R2_001_val_2.fq.gz -S s044.bt2.sam --no-unal --al-conc ./s044.al --un-conc symbionts/s044.un</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s045_R1_001_val_1.fq.gz -2 s045_R2_001_val_2.fq.gz -S s045.bt2.sam --no-unal --al ./s045.al --un symbionts/s045.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s045_R1_001_val_1.fq.gz -2 s045_R2_001_val_2.fq.gz -S s045.bt2.sam --no-unal --al-conc ./s045.al --un-conc symbionts/s045.un</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -7786,7 +7786,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s046_R1_001_val_1.fq.gz -2 s046_R2_001_val_2.fq.gz -S s046.bt2.sam --no-unal --al ./s046.al --un symbionts/s046.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s046_R1_001_val_1.fq.gz -2 s046_R2_001_val_2.fq.gz -S s046.bt2.sam --no-unal --al-conc ./s046.al --un-conc symbionts/s046.un</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -7801,7 +7801,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s047_R1_001_val_1.fq.gz -2 s047_R2_001_val_2.fq.gz -S s047.bt2.sam --no-unal --al ./s047.al --un symbionts/s047.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s047_R1_001_val_1.fq.gz -2 s047_R2_001_val_2.fq.gz -S s047.bt2.sam --no-unal --al-conc ./s047.al --un-conc symbionts/s047.un</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -7816,7 +7816,7 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s048_R1_001_val_1.fq.gz -2 s048_R2_001_val_2.fq.gz -S s048.bt2.sam --no-unal --al ./s048.al --un symbionts/s048.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s048_R1_001_val_1.fq.gz -2 s048_R2_001_val_2.fq.gz -S s048.bt2.sam --no-unal --al-conc ./s048.al --un-conc symbionts/s048.un</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -7831,7 +7831,7 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s049_R1_001_val_1.fq.gz -2 s049_R2_001_val_2.fq.gz -S s049.bt2.sam --no-unal --al ./s049.al --un symbionts/s049.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s049_R1_001_val_1.fq.gz -2 s049_R2_001_val_2.fq.gz -S s049.bt2.sam --no-unal --al-conc ./s049.al --un-conc symbionts/s049.un</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -7846,7 +7846,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s050_R1_001_val_1.fq.gz -2 s050_R2_001_val_2.fq.gz -S s050.bt2.sam --no-unal --al ./s050.al --un symbionts/s050.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s050_R1_001_val_1.fq.gz -2 s050_R2_001_val_2.fq.gz -S s050.bt2.sam --no-unal --al-conc ./s050.al --un-conc symbionts/s050.un</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s051_R1_001_val_1.fq.gz -2 s051_R2_001_val_2.fq.gz -S s051.bt2.sam --no-unal --al ./s051.al --un symbionts/s051.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s051_R1_001_val_1.fq.gz -2 s051_R2_001_val_2.fq.gz -S s051.bt2.sam --no-unal --al-conc ./s051.al --un-conc symbionts/s051.un</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -7876,7 +7876,7 @@
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s052_R1_001_val_1.fq.gz -2 s052_R2_001_val_2.fq.gz -S s052.bt2.sam --no-unal --al ./s052.al --un symbionts/s052.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s052_R1_001_val_1.fq.gz -2 s052_R2_001_val_2.fq.gz -S s052.bt2.sam --no-unal --al-conc ./s052.al --un-conc symbionts/s052.un</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -7891,7 +7891,7 @@
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s053_R1_001_val_1.fq.gz -2 s053_R2_001_val_2.fq.gz -S s053.bt2.sam --no-unal --al ./s053.al --un symbionts/s053.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s053_R1_001_val_1.fq.gz -2 s053_R2_001_val_2.fq.gz -S s053.bt2.sam --no-unal --al-conc ./s053.al --un-conc symbionts/s053.un</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -7906,7 +7906,7 @@
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s054_R1_001_val_1.fq.gz -2 s054_R2_001_val_2.fq.gz -S s054.bt2.sam --no-unal --al ./s054.al --un symbionts/s054.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s054_R1_001_val_1.fq.gz -2 s054_R2_001_val_2.fq.gz -S s054.bt2.sam --no-unal --al-conc ./s054.al --un-conc symbionts/s054.un</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s055_R1_001_val_1.fq.gz -2 s055_R2_001_val_2.fq.gz -S s055.bt2.sam --no-unal --al ./s055.al --un symbionts/s055.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s055_R1_001_val_1.fq.gz -2 s055_R2_001_val_2.fq.gz -S s055.bt2.sam --no-unal --al-conc ./s055.al --un-conc symbionts/s055.un</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -7936,7 +7936,7 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s056_R1_001_val_1.fq.gz -2 s056_R2_001_val_2.fq.gz -S s056.bt2.sam --no-unal --al ./s056.al --un symbionts/s056.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s056_R1_001_val_1.fq.gz -2 s056_R2_001_val_2.fq.gz -S s056.bt2.sam --no-unal --al-conc ./s056.al --un-conc symbionts/s056.un</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -7951,7 +7951,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s057_R1_001_val_1.fq.gz -2 s057_R2_001_val_2.fq.gz -S s057.bt2.sam --no-unal --al ./s057.al --un symbionts/s057.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s057_R1_001_val_1.fq.gz -2 s057_R2_001_val_2.fq.gz -S s057.bt2.sam --no-unal --al-conc ./s057.al --un-conc symbionts/s057.un</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -7966,7 +7966,7 @@
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s058_R1_001_val_1.fq.gz -2 s058_R2_001_val_2.fq.gz -S s058.bt2.sam --no-unal --al ./s058.al --un symbionts/s058.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s058_R1_001_val_1.fq.gz -2 s058_R2_001_val_2.fq.gz -S s058.bt2.sam --no-unal --al-conc ./s058.al --un-conc symbionts/s058.un</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -7981,7 +7981,7 @@
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s059_R1_001_val_1.fq.gz -2 s059_R2_001_val_2.fq.gz -S s059.bt2.sam --no-unal --al ./s059.al --un symbionts/s059.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s059_R1_001_val_1.fq.gz -2 s059_R2_001_val_2.fq.gz -S s059.bt2.sam --no-unal --al-conc ./s059.al --un-conc symbionts/s059.un</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -7996,7 +7996,7 @@
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s060_R1_001_val_1.fq.gz -2 s060_R2_001_val_2.fq.gz -S s060.bt2.sam --no-unal --al ./s060.al --un symbionts/s060.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s060_R1_001_val_1.fq.gz -2 s060_R2_001_val_2.fq.gz -S s060.bt2.sam --no-unal --al-conc ./s060.al --un-conc symbionts/s060.un</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s061_R1_001_val_1.fq.gz -2 s061_R2_001_val_2.fq.gz -S s061.bt2.sam --no-unal --al ./s061.al --un symbionts/s061.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s061_R1_001_val_1.fq.gz -2 s061_R2_001_val_2.fq.gz -S s061.bt2.sam --no-unal --al-conc ./s061.al --un-conc symbionts/s061.un</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -8026,7 +8026,7 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s062_R1_001_val_1.fq.gz -2 s062_R2_001_val_2.fq.gz -S s062.bt2.sam --no-unal --al ./s062.al --un symbionts/s062.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s062_R1_001_val_1.fq.gz -2 s062_R2_001_val_2.fq.gz -S s062.bt2.sam --no-unal --al-conc ./s062.al --un-conc symbionts/s062.un</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s063_R1_001_val_1.fq.gz -2 s063_R2_001_val_2.fq.gz -S s063.bt2.sam --no-unal --al ./s063.al --un symbionts/s063.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s063_R1_001_val_1.fq.gz -2 s063_R2_001_val_2.fq.gz -S s063.bt2.sam --no-unal --al-conc ./s063.al --un-conc symbionts/s063.un</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -8056,7 +8056,7 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s064_R1_001_val_1.fq.gz -2 s064_R2_001_val_2.fq.gz -S s064.bt2.sam --no-unal --al ./s064.al --un symbionts/s064.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s064_R1_001_val_1.fq.gz -2 s064_R2_001_val_2.fq.gz -S s064.bt2.sam --no-unal --al-conc ./s064.al --un-conc symbionts/s064.un</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -8071,7 +8071,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s065_R1_001_val_1.fq.gz -2 s065_R2_001_val_2.fq.gz -S s065.bt2.sam --no-unal --al ./s065.al --un symbionts/s065.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s065_R1_001_val_1.fq.gz -2 s065_R2_001_val_2.fq.gz -S s065.bt2.sam --no-unal --al-conc ./s065.al --un-conc symbionts/s065.un</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -8085,8 +8085,8 @@
         <v>785</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" ref="H66:H129" si="1">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A66&amp;" -2 "&amp;C66&amp;" -S "&amp;F66&amp;".bt2.sam --no-unal --al ./"&amp;F66&amp;".al --un symbionts/"&amp;F66&amp;".un"</f>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s066_R1_001_val_1.fq.gz -2 s066_R2_001_val_2.fq.gz -S s066.bt2.sam --no-unal --al ./s066.al --un symbionts/s066.un</v>
+        <f t="shared" ref="H66:H129" si="1">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A66&amp;" -2 "&amp;C66&amp;" -S "&amp;F66&amp;".bt2.sam --no-unal --al-conc ./"&amp;F66&amp;".al --un-conc symbionts/"&amp;F66&amp;".un"</f>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s066_R1_001_val_1.fq.gz -2 s066_R2_001_val_2.fq.gz -S s066.bt2.sam --no-unal --al-conc ./s066.al --un-conc symbionts/s066.un</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -8101,7 +8101,7 @@
       </c>
       <c r="H67" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s067_R1_001_val_1.fq.gz -2 s067_R2_001_val_2.fq.gz -S s067.bt2.sam --no-unal --al ./s067.al --un symbionts/s067.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s067_R1_001_val_1.fq.gz -2 s067_R2_001_val_2.fq.gz -S s067.bt2.sam --no-unal --al-conc ./s067.al --un-conc symbionts/s067.un</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -8116,7 +8116,7 @@
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s068_R1_001_val_1.fq.gz -2 s068_R2_001_val_2.fq.gz -S s068.bt2.sam --no-unal --al ./s068.al --un symbionts/s068.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s068_R1_001_val_1.fq.gz -2 s068_R2_001_val_2.fq.gz -S s068.bt2.sam --no-unal --al-conc ./s068.al --un-conc symbionts/s068.un</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s069_R1_001_val_1.fq.gz -2 s069_R2_001_val_2.fq.gz -S s069.bt2.sam --no-unal --al ./s069.al --un symbionts/s069.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s069_R1_001_val_1.fq.gz -2 s069_R2_001_val_2.fq.gz -S s069.bt2.sam --no-unal --al-conc ./s069.al --un-conc symbionts/s069.un</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -8146,7 +8146,7 @@
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s070_R1_001_val_1.fq.gz -2 s070_R2_001_val_2.fq.gz -S s070.bt2.sam --no-unal --al ./s070.al --un symbionts/s070.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s070_R1_001_val_1.fq.gz -2 s070_R2_001_val_2.fq.gz -S s070.bt2.sam --no-unal --al-conc ./s070.al --un-conc symbionts/s070.un</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s071_R1_001_val_1.fq.gz -2 s071_R2_001_val_2.fq.gz -S s071.bt2.sam --no-unal --al ./s071.al --un symbionts/s071.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s071_R1_001_val_1.fq.gz -2 s071_R2_001_val_2.fq.gz -S s071.bt2.sam --no-unal --al-conc ./s071.al --un-conc symbionts/s071.un</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -8176,7 +8176,7 @@
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s072_R1_001_val_1.fq.gz -2 s072_R2_001_val_2.fq.gz -S s072.bt2.sam --no-unal --al ./s072.al --un symbionts/s072.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s072_R1_001_val_1.fq.gz -2 s072_R2_001_val_2.fq.gz -S s072.bt2.sam --no-unal --al-conc ./s072.al --un-conc symbionts/s072.un</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -8191,7 +8191,7 @@
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s073_R1_001_val_1.fq.gz -2 s073_R2_001_val_2.fq.gz -S s073.bt2.sam --no-unal --al ./s073.al --un symbionts/s073.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s073_R1_001_val_1.fq.gz -2 s073_R2_001_val_2.fq.gz -S s073.bt2.sam --no-unal --al-conc ./s073.al --un-conc symbionts/s073.un</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -8206,7 +8206,7 @@
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s074_R1_001_val_1.fq.gz -2 s074_R2_001_val_2.fq.gz -S s074.bt2.sam --no-unal --al ./s074.al --un symbionts/s074.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s074_R1_001_val_1.fq.gz -2 s074_R2_001_val_2.fq.gz -S s074.bt2.sam --no-unal --al-conc ./s074.al --un-conc symbionts/s074.un</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -8221,7 +8221,7 @@
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s075_R1_001_val_1.fq.gz -2 s075_R2_001_val_2.fq.gz -S s075.bt2.sam --no-unal --al ./s075.al --un symbionts/s075.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s075_R1_001_val_1.fq.gz -2 s075_R2_001_val_2.fq.gz -S s075.bt2.sam --no-unal --al-conc ./s075.al --un-conc symbionts/s075.un</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s076_R1_001_val_1.fq.gz -2 s076_R2_001_val_2.fq.gz -S s076.bt2.sam --no-unal --al ./s076.al --un symbionts/s076.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s076_R1_001_val_1.fq.gz -2 s076_R2_001_val_2.fq.gz -S s076.bt2.sam --no-unal --al-conc ./s076.al --un-conc symbionts/s076.un</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -8251,7 +8251,7 @@
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s077_R1_001_val_1.fq.gz -2 s077_R2_001_val_2.fq.gz -S s077.bt2.sam --no-unal --al ./s077.al --un symbionts/s077.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s077_R1_001_val_1.fq.gz -2 s077_R2_001_val_2.fq.gz -S s077.bt2.sam --no-unal --al-conc ./s077.al --un-conc symbionts/s077.un</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -8266,7 +8266,7 @@
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s078_R1_001_val_1.fq.gz -2 s078_R2_001_val_2.fq.gz -S s078.bt2.sam --no-unal --al ./s078.al --un symbionts/s078.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s078_R1_001_val_1.fq.gz -2 s078_R2_001_val_2.fq.gz -S s078.bt2.sam --no-unal --al-conc ./s078.al --un-conc symbionts/s078.un</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -8281,7 +8281,7 @@
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s079_R1_001_val_1.fq.gz -2 s079_R2_001_val_2.fq.gz -S s079.bt2.sam --no-unal --al ./s079.al --un symbionts/s079.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s079_R1_001_val_1.fq.gz -2 s079_R2_001_val_2.fq.gz -S s079.bt2.sam --no-unal --al-conc ./s079.al --un-conc symbionts/s079.un</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s080_R1_001_val_1.fq.gz -2 s080_R2_001_val_2.fq.gz -S s080.bt2.sam --no-unal --al ./s080.al --un symbionts/s080.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s080_R1_001_val_1.fq.gz -2 s080_R2_001_val_2.fq.gz -S s080.bt2.sam --no-unal --al-conc ./s080.al --un-conc symbionts/s080.un</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -8311,7 +8311,7 @@
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s081_R1_001_val_1.fq.gz -2 s081_R2_001_val_2.fq.gz -S s081.bt2.sam --no-unal --al ./s081.al --un symbionts/s081.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s081_R1_001_val_1.fq.gz -2 s081_R2_001_val_2.fq.gz -S s081.bt2.sam --no-unal --al-conc ./s081.al --un-conc symbionts/s081.un</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -8326,7 +8326,7 @@
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s082_R1_001_val_1.fq.gz -2 s082_R2_001_val_2.fq.gz -S s082.bt2.sam --no-unal --al ./s082.al --un symbionts/s082.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s082_R1_001_val_1.fq.gz -2 s082_R2_001_val_2.fq.gz -S s082.bt2.sam --no-unal --al-conc ./s082.al --un-conc symbionts/s082.un</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s083_R1_001_val_1.fq.gz -2 s083_R2_001_val_2.fq.gz -S s083.bt2.sam --no-unal --al ./s083.al --un symbionts/s083.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s083_R1_001_val_1.fq.gz -2 s083_R2_001_val_2.fq.gz -S s083.bt2.sam --no-unal --al-conc ./s083.al --un-conc symbionts/s083.un</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -8356,7 +8356,7 @@
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s084_R1_001_val_1.fq.gz -2 s084_R2_001_val_2.fq.gz -S s084.bt2.sam --no-unal --al ./s084.al --un symbionts/s084.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s084_R1_001_val_1.fq.gz -2 s084_R2_001_val_2.fq.gz -S s084.bt2.sam --no-unal --al-conc ./s084.al --un-conc symbionts/s084.un</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s085_R1_001_val_1.fq.gz -2 s085_R2_001_val_2.fq.gz -S s085.bt2.sam --no-unal --al ./s085.al --un symbionts/s085.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s085_R1_001_val_1.fq.gz -2 s085_R2_001_val_2.fq.gz -S s085.bt2.sam --no-unal --al-conc ./s085.al --un-conc symbionts/s085.un</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -8386,7 +8386,7 @@
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s086_R1_001_val_1.fq.gz -2 s086_R2_001_val_2.fq.gz -S s086.bt2.sam --no-unal --al ./s086.al --un symbionts/s086.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s086_R1_001_val_1.fq.gz -2 s086_R2_001_val_2.fq.gz -S s086.bt2.sam --no-unal --al-conc ./s086.al --un-conc symbionts/s086.un</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s087_R1_001_val_1.fq.gz -2 s087_R2_001_val_2.fq.gz -S s087.bt2.sam --no-unal --al ./s087.al --un symbionts/s087.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s087_R1_001_val_1.fq.gz -2 s087_R2_001_val_2.fq.gz -S s087.bt2.sam --no-unal --al-conc ./s087.al --un-conc symbionts/s087.un</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -8416,7 +8416,7 @@
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s088_R1_001_val_1.fq.gz -2 s088_R2_001_val_2.fq.gz -S s088.bt2.sam --no-unal --al ./s088.al --un symbionts/s088.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s088_R1_001_val_1.fq.gz -2 s088_R2_001_val_2.fq.gz -S s088.bt2.sam --no-unal --al-conc ./s088.al --un-conc symbionts/s088.un</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s089_R1_001_val_1.fq.gz -2 s089_R2_001_val_2.fq.gz -S s089.bt2.sam --no-unal --al ./s089.al --un symbionts/s089.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s089_R1_001_val_1.fq.gz -2 s089_R2_001_val_2.fq.gz -S s089.bt2.sam --no-unal --al-conc ./s089.al --un-conc symbionts/s089.un</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -8446,7 +8446,7 @@
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s090_R1_001_val_1.fq.gz -2 s090_R2_001_val_2.fq.gz -S s090.bt2.sam --no-unal --al ./s090.al --un symbionts/s090.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s090_R1_001_val_1.fq.gz -2 s090_R2_001_val_2.fq.gz -S s090.bt2.sam --no-unal --al-conc ./s090.al --un-conc symbionts/s090.un</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s091_R1_001_val_1.fq.gz -2 s091_R2_001_val_2.fq.gz -S s091.bt2.sam --no-unal --al ./s091.al --un symbionts/s091.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s091_R1_001_val_1.fq.gz -2 s091_R2_001_val_2.fq.gz -S s091.bt2.sam --no-unal --al-conc ./s091.al --un-conc symbionts/s091.un</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="H92" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s092_R1_001_val_1.fq.gz -2 s092_R2_001_val_2.fq.gz -S s092.bt2.sam --no-unal --al ./s092.al --un symbionts/s092.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s092_R1_001_val_1.fq.gz -2 s092_R2_001_val_2.fq.gz -S s092.bt2.sam --no-unal --al-conc ./s092.al --un-conc symbionts/s092.un</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -8491,7 +8491,7 @@
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s093_R1_001_val_1.fq.gz -2 s093_R2_001_val_2.fq.gz -S s093.bt2.sam --no-unal --al ./s093.al --un symbionts/s093.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s093_R1_001_val_1.fq.gz -2 s093_R2_001_val_2.fq.gz -S s093.bt2.sam --no-unal --al-conc ./s093.al --un-conc symbionts/s093.un</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -8506,7 +8506,7 @@
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s094_R1_001_val_1.fq.gz -2 s094_R2_001_val_2.fq.gz -S s094.bt2.sam --no-unal --al ./s094.al --un symbionts/s094.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s094_R1_001_val_1.fq.gz -2 s094_R2_001_val_2.fq.gz -S s094.bt2.sam --no-unal --al-conc ./s094.al --un-conc symbionts/s094.un</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -8521,7 +8521,7 @@
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s095_R1_001_val_1.fq.gz -2 s095_R2_001_val_2.fq.gz -S s095.bt2.sam --no-unal --al ./s095.al --un symbionts/s095.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s095_R1_001_val_1.fq.gz -2 s095_R2_001_val_2.fq.gz -S s095.bt2.sam --no-unal --al-conc ./s095.al --un-conc symbionts/s095.un</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -8536,7 +8536,7 @@
       </c>
       <c r="H96" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s096_R1_001_val_1.fq.gz -2 s096_R2_001_val_2.fq.gz -S s096.bt2.sam --no-unal --al ./s096.al --un symbionts/s096.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s096_R1_001_val_1.fq.gz -2 s096_R2_001_val_2.fq.gz -S s096.bt2.sam --no-unal --al-conc ./s096.al --un-conc symbionts/s096.un</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s097_R1_001_val_1.fq.gz -2 s097_R2_001_val_2.fq.gz -S s097.bt2.sam --no-unal --al ./s097.al --un symbionts/s097.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s097_R1_001_val_1.fq.gz -2 s097_R2_001_val_2.fq.gz -S s097.bt2.sam --no-unal --al-conc ./s097.al --un-conc symbionts/s097.un</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -8566,7 +8566,7 @@
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s098_R1_001_val_1.fq.gz -2 s098_R2_001_val_2.fq.gz -S s098.bt2.sam --no-unal --al ./s098.al --un symbionts/s098.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s098_R1_001_val_1.fq.gz -2 s098_R2_001_val_2.fq.gz -S s098.bt2.sam --no-unal --al-conc ./s098.al --un-conc symbionts/s098.un</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -8581,7 +8581,7 @@
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s099_R1_001_val_1.fq.gz -2 s099_R2_001_val_2.fq.gz -S s099.bt2.sam --no-unal --al ./s099.al --un symbionts/s099.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s099_R1_001_val_1.fq.gz -2 s099_R2_001_val_2.fq.gz -S s099.bt2.sam --no-unal --al-conc ./s099.al --un-conc symbionts/s099.un</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -8596,7 +8596,7 @@
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s100_R1_001_val_1.fq.gz -2 s100_R2_001_val_2.fq.gz -S s100.bt2.sam --no-unal --al ./s100.al --un symbionts/s100.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s100_R1_001_val_1.fq.gz -2 s100_R2_001_val_2.fq.gz -S s100.bt2.sam --no-unal --al-conc ./s100.al --un-conc symbionts/s100.un</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s101_R1_001_val_1.fq.gz -2 s101_R2_001_val_2.fq.gz -S s101.bt2.sam --no-unal --al ./s101.al --un symbionts/s101.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s101_R1_001_val_1.fq.gz -2 s101_R2_001_val_2.fq.gz -S s101.bt2.sam --no-unal --al-conc ./s101.al --un-conc symbionts/s101.un</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -8626,7 +8626,7 @@
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s102_R1_001_val_1.fq.gz -2 s102_R2_001_val_2.fq.gz -S s102.bt2.sam --no-unal --al ./s102.al --un symbionts/s102.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s102_R1_001_val_1.fq.gz -2 s102_R2_001_val_2.fq.gz -S s102.bt2.sam --no-unal --al-conc ./s102.al --un-conc symbionts/s102.un</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -8641,7 +8641,7 @@
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s103_R1_001_val_1.fq.gz -2 s103_R2_001_val_2.fq.gz -S s103.bt2.sam --no-unal --al ./s103.al --un symbionts/s103.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s103_R1_001_val_1.fq.gz -2 s103_R2_001_val_2.fq.gz -S s103.bt2.sam --no-unal --al-conc ./s103.al --un-conc symbionts/s103.un</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -8656,7 +8656,7 @@
       </c>
       <c r="H104" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s104_R1_001_val_1.fq.gz -2 s104_R2_001_val_2.fq.gz -S s104.bt2.sam --no-unal --al ./s104.al --un symbionts/s104.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s104_R1_001_val_1.fq.gz -2 s104_R2_001_val_2.fq.gz -S s104.bt2.sam --no-unal --al-conc ./s104.al --un-conc symbionts/s104.un</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -8671,7 +8671,7 @@
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s105_R1_001_val_1.fq.gz -2 s105_R2_001_val_2.fq.gz -S s105.bt2.sam --no-unal --al ./s105.al --un symbionts/s105.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s105_R1_001_val_1.fq.gz -2 s105_R2_001_val_2.fq.gz -S s105.bt2.sam --no-unal --al-conc ./s105.al --un-conc symbionts/s105.un</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s106_R1_001_val_1.fq.gz -2 s106_R2_001_val_2.fq.gz -S s106.bt2.sam --no-unal --al ./s106.al --un symbionts/s106.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s106_R1_001_val_1.fq.gz -2 s106_R2_001_val_2.fq.gz -S s106.bt2.sam --no-unal --al-conc ./s106.al --un-conc symbionts/s106.un</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -8701,7 +8701,7 @@
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s107_R1_001_val_1.fq.gz -2 s107_R2_001_val_2.fq.gz -S s107.bt2.sam --no-unal --al ./s107.al --un symbionts/s107.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s107_R1_001_val_1.fq.gz -2 s107_R2_001_val_2.fq.gz -S s107.bt2.sam --no-unal --al-conc ./s107.al --un-conc symbionts/s107.un</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -8716,7 +8716,7 @@
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s108_R1_001_val_1.fq.gz -2 s108_R2_001_val_2.fq.gz -S s108.bt2.sam --no-unal --al ./s108.al --un symbionts/s108.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s108_R1_001_val_1.fq.gz -2 s108_R2_001_val_2.fq.gz -S s108.bt2.sam --no-unal --al-conc ./s108.al --un-conc symbionts/s108.un</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s109_R1_001_val_1.fq.gz -2 s109_R2_001_val_2.fq.gz -S s109.bt2.sam --no-unal --al ./s109.al --un symbionts/s109.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s109_R1_001_val_1.fq.gz -2 s109_R2_001_val_2.fq.gz -S s109.bt2.sam --no-unal --al-conc ./s109.al --un-conc symbionts/s109.un</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -8746,7 +8746,7 @@
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s110_R1_001_val_1.fq.gz -2 s110_R2_001_val_2.fq.gz -S s110.bt2.sam --no-unal --al ./s110.al --un symbionts/s110.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s110_R1_001_val_1.fq.gz -2 s110_R2_001_val_2.fq.gz -S s110.bt2.sam --no-unal --al-conc ./s110.al --un-conc symbionts/s110.un</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s111_R1_001_val_1.fq.gz -2 s111_R2_001_val_2.fq.gz -S s111.bt2.sam --no-unal --al ./s111.al --un symbionts/s111.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s111_R1_001_val_1.fq.gz -2 s111_R2_001_val_2.fq.gz -S s111.bt2.sam --no-unal --al-conc ./s111.al --un-conc symbionts/s111.un</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -8776,7 +8776,7 @@
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s112_R1_001_val_1.fq.gz -2 s112_R2_001_val_2.fq.gz -S s112.bt2.sam --no-unal --al ./s112.al --un symbionts/s112.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s112_R1_001_val_1.fq.gz -2 s112_R2_001_val_2.fq.gz -S s112.bt2.sam --no-unal --al-conc ./s112.al --un-conc symbionts/s112.un</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -8791,7 +8791,7 @@
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s113_R1_001_val_1.fq.gz -2 s113_R2_001_val_2.fq.gz -S s113.bt2.sam --no-unal --al ./s113.al --un symbionts/s113.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s113_R1_001_val_1.fq.gz -2 s113_R2_001_val_2.fq.gz -S s113.bt2.sam --no-unal --al-conc ./s113.al --un-conc symbionts/s113.un</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -8806,7 +8806,7 @@
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s114_R1_001_val_1.fq.gz -2 s114_R2_001_val_2.fq.gz -S s114.bt2.sam --no-unal --al ./s114.al --un symbionts/s114.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s114_R1_001_val_1.fq.gz -2 s114_R2_001_val_2.fq.gz -S s114.bt2.sam --no-unal --al-conc ./s114.al --un-conc symbionts/s114.un</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s115_R1_001_val_1.fq.gz -2 s115_R2_001_val_2.fq.gz -S s115.bt2.sam --no-unal --al ./s115.al --un symbionts/s115.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s115_R1_001_val_1.fq.gz -2 s115_R2_001_val_2.fq.gz -S s115.bt2.sam --no-unal --al-conc ./s115.al --un-conc symbionts/s115.un</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -8836,7 +8836,7 @@
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s116_R1_001_val_1.fq.gz -2 s116_R2_001_val_2.fq.gz -S s116.bt2.sam --no-unal --al ./s116.al --un symbionts/s116.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s116_R1_001_val_1.fq.gz -2 s116_R2_001_val_2.fq.gz -S s116.bt2.sam --no-unal --al-conc ./s116.al --un-conc symbionts/s116.un</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -8851,7 +8851,7 @@
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s117_R1_001_val_1.fq.gz -2 s117_R2_001_val_2.fq.gz -S s117.bt2.sam --no-unal --al ./s117.al --un symbionts/s117.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s117_R1_001_val_1.fq.gz -2 s117_R2_001_val_2.fq.gz -S s117.bt2.sam --no-unal --al-conc ./s117.al --un-conc symbionts/s117.un</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -8866,7 +8866,7 @@
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s118_R1_001_val_1.fq.gz -2 s118_R2_001_val_2.fq.gz -S s118.bt2.sam --no-unal --al ./s118.al --un symbionts/s118.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s118_R1_001_val_1.fq.gz -2 s118_R2_001_val_2.fq.gz -S s118.bt2.sam --no-unal --al-conc ./s118.al --un-conc symbionts/s118.un</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -8881,7 +8881,7 @@
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s119_R1_001_val_1.fq.gz -2 s119_R2_001_val_2.fq.gz -S s119.bt2.sam --no-unal --al ./s119.al --un symbionts/s119.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s119_R1_001_val_1.fq.gz -2 s119_R2_001_val_2.fq.gz -S s119.bt2.sam --no-unal --al-conc ./s119.al --un-conc symbionts/s119.un</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -8896,7 +8896,7 @@
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s120_R1_001_val_1.fq.gz -2 s120_R2_001_val_2.fq.gz -S s120.bt2.sam --no-unal --al ./s120.al --un symbionts/s120.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s120_R1_001_val_1.fq.gz -2 s120_R2_001_val_2.fq.gz -S s120.bt2.sam --no-unal --al-conc ./s120.al --un-conc symbionts/s120.un</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s121_R1_001_val_1.fq.gz -2 s121_R2_001_val_2.fq.gz -S s121.bt2.sam --no-unal --al ./s121.al --un symbionts/s121.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s121_R1_001_val_1.fq.gz -2 s121_R2_001_val_2.fq.gz -S s121.bt2.sam --no-unal --al-conc ./s121.al --un-conc symbionts/s121.un</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -8926,7 +8926,7 @@
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s122_R1_001_val_1.fq.gz -2 s122_R2_001_val_2.fq.gz -S s122.bt2.sam --no-unal --al ./s122.al --un symbionts/s122.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s122_R1_001_val_1.fq.gz -2 s122_R2_001_val_2.fq.gz -S s122.bt2.sam --no-unal --al-conc ./s122.al --un-conc symbionts/s122.un</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s123_R1_001_val_1.fq.gz -2 s123_R2_001_val_2.fq.gz -S s123.bt2.sam --no-unal --al ./s123.al --un symbionts/s123.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s123_R1_001_val_1.fq.gz -2 s123_R2_001_val_2.fq.gz -S s123.bt2.sam --no-unal --al-conc ./s123.al --un-conc symbionts/s123.un</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -8956,7 +8956,7 @@
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s124_R1_001_val_1.fq.gz -2 s124_R2_001_val_2.fq.gz -S s124.bt2.sam --no-unal --al ./s124.al --un symbionts/s124.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s124_R1_001_val_1.fq.gz -2 s124_R2_001_val_2.fq.gz -S s124.bt2.sam --no-unal --al-conc ./s124.al --un-conc symbionts/s124.un</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="H125" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s125_R1_001_val_1.fq.gz -2 s125_R2_001_val_2.fq.gz -S s125.bt2.sam --no-unal --al ./s125.al --un symbionts/s125.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s125_R1_001_val_1.fq.gz -2 s125_R2_001_val_2.fq.gz -S s125.bt2.sam --no-unal --al-conc ./s125.al --un-conc symbionts/s125.un</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -8986,7 +8986,7 @@
       </c>
       <c r="H126" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s126_R1_001_val_1.fq.gz -2 s126_R2_001_val_2.fq.gz -S s126.bt2.sam --no-unal --al ./s126.al --un symbionts/s126.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s126_R1_001_val_1.fq.gz -2 s126_R2_001_val_2.fq.gz -S s126.bt2.sam --no-unal --al-conc ./s126.al --un-conc symbionts/s126.un</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="H127" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s127_R1_001_val_1.fq.gz -2 s127_R2_001_val_2.fq.gz -S s127.bt2.sam --no-unal --al ./s127.al --un symbionts/s127.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s127_R1_001_val_1.fq.gz -2 s127_R2_001_val_2.fq.gz -S s127.bt2.sam --no-unal --al-conc ./s127.al --un-conc symbionts/s127.un</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -9016,7 +9016,7 @@
       </c>
       <c r="H128" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s128_R1_001_val_1.fq.gz -2 s128_R2_001_val_2.fq.gz -S s128.bt2.sam --no-unal --al ./s128.al --un symbionts/s128.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s128_R1_001_val_1.fq.gz -2 s128_R2_001_val_2.fq.gz -S s128.bt2.sam --no-unal --al-conc ./s128.al --un-conc symbionts/s128.un</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -9031,7 +9031,7 @@
       </c>
       <c r="H129" t="str">
         <f t="shared" si="1"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s129_R1_001_val_1.fq.gz -2 s129_R2_001_val_2.fq.gz -S s129.bt2.sam --no-unal --al ./s129.al --un symbionts/s129.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s129_R1_001_val_1.fq.gz -2 s129_R2_001_val_2.fq.gz -S s129.bt2.sam --no-unal --al-conc ./s129.al --un-conc symbionts/s129.un</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -9045,8 +9045,8 @@
         <v>849</v>
       </c>
       <c r="H130" t="str">
-        <f t="shared" ref="H130:H180" si="2">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A130&amp;" -2 "&amp;C130&amp;" -S "&amp;F130&amp;".bt2.sam --no-unal --al ./"&amp;F130&amp;".al --un symbionts/"&amp;F130&amp;".un"</f>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s130_R1_001_val_1.fq.gz -2 s130_R2_001_val_2.fq.gz -S s130.bt2.sam --no-unal --al ./s130.al --un symbionts/s130.un</v>
+        <f t="shared" ref="H130:H180" si="2">"bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 "&amp;A130&amp;" -2 "&amp;C130&amp;" -S "&amp;F130&amp;".bt2.sam --no-unal --al-conc ./"&amp;F130&amp;".al --un-conc symbionts/"&amp;F130&amp;".un"</f>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s130_R1_001_val_1.fq.gz -2 s130_R2_001_val_2.fq.gz -S s130.bt2.sam --no-unal --al-conc ./s130.al --un-conc symbionts/s130.un</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -9061,7 +9061,7 @@
       </c>
       <c r="H131" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s131_R1_001_val_1.fq.gz -2 s131_R2_001_val_2.fq.gz -S s131.bt2.sam --no-unal --al ./s131.al --un symbionts/s131.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s131_R1_001_val_1.fq.gz -2 s131_R2_001_val_2.fq.gz -S s131.bt2.sam --no-unal --al-conc ./s131.al --un-conc symbionts/s131.un</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -9076,7 +9076,7 @@
       </c>
       <c r="H132" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s132_R1_001_val_1.fq.gz -2 s132_R2_001_val_2.fq.gz -S s132.bt2.sam --no-unal --al ./s132.al --un symbionts/s132.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s132_R1_001_val_1.fq.gz -2 s132_R2_001_val_2.fq.gz -S s132.bt2.sam --no-unal --al-conc ./s132.al --un-conc symbionts/s132.un</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -9091,7 +9091,7 @@
       </c>
       <c r="H133" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s133_R1_001_val_1.fq.gz -2 s133_R2_001_val_2.fq.gz -S s133.bt2.sam --no-unal --al ./s133.al --un symbionts/s133.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s133_R1_001_val_1.fq.gz -2 s133_R2_001_val_2.fq.gz -S s133.bt2.sam --no-unal --al-conc ./s133.al --un-conc symbionts/s133.un</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -9106,7 +9106,7 @@
       </c>
       <c r="H134" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s134_R1_001_val_1.fq.gz -2 s134_R2_001_val_2.fq.gz -S s134.bt2.sam --no-unal --al ./s134.al --un symbionts/s134.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s134_R1_001_val_1.fq.gz -2 s134_R2_001_val_2.fq.gz -S s134.bt2.sam --no-unal --al-conc ./s134.al --un-conc symbionts/s134.un</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -9121,7 +9121,7 @@
       </c>
       <c r="H135" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s135_R1_001_val_1.fq.gz -2 s135_R2_001_val_2.fq.gz -S s135.bt2.sam --no-unal --al ./s135.al --un symbionts/s135.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s135_R1_001_val_1.fq.gz -2 s135_R2_001_val_2.fq.gz -S s135.bt2.sam --no-unal --al-conc ./s135.al --un-conc symbionts/s135.un</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -9136,7 +9136,7 @@
       </c>
       <c r="H136" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s136_R1_001_val_1.fq.gz -2 s136_R2_001_val_2.fq.gz -S s136.bt2.sam --no-unal --al ./s136.al --un symbionts/s136.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s136_R1_001_val_1.fq.gz -2 s136_R2_001_val_2.fq.gz -S s136.bt2.sam --no-unal --al-conc ./s136.al --un-conc symbionts/s136.un</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -9151,7 +9151,7 @@
       </c>
       <c r="H137" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s137_R1_001_val_1.fq.gz -2 s137_R2_001_val_2.fq.gz -S s137.bt2.sam --no-unal --al ./s137.al --un symbionts/s137.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s137_R1_001_val_1.fq.gz -2 s137_R2_001_val_2.fq.gz -S s137.bt2.sam --no-unal --al-conc ./s137.al --un-conc symbionts/s137.un</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -9166,7 +9166,7 @@
       </c>
       <c r="H138" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s138_R1_001_val_1.fq.gz -2 s138_R2_001_val_2.fq.gz -S s138.bt2.sam --no-unal --al ./s138.al --un symbionts/s138.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s138_R1_001_val_1.fq.gz -2 s138_R2_001_val_2.fq.gz -S s138.bt2.sam --no-unal --al-conc ./s138.al --un-conc symbionts/s138.un</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -9181,7 +9181,7 @@
       </c>
       <c r="H139" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s139_R1_001_val_1.fq.gz -2 s139_R2_001_val_2.fq.gz -S s139.bt2.sam --no-unal --al ./s139.al --un symbionts/s139.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s139_R1_001_val_1.fq.gz -2 s139_R2_001_val_2.fq.gz -S s139.bt2.sam --no-unal --al-conc ./s139.al --un-conc symbionts/s139.un</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -9196,7 +9196,7 @@
       </c>
       <c r="H140" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s140_R1_001_val_1.fq.gz -2 s140_R2_001_val_2.fq.gz -S s140.bt2.sam --no-unal --al ./s140.al --un symbionts/s140.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s140_R1_001_val_1.fq.gz -2 s140_R2_001_val_2.fq.gz -S s140.bt2.sam --no-unal --al-conc ./s140.al --un-conc symbionts/s140.un</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="H141" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s141_R1_001_val_1.fq.gz -2 s141_R2_001_val_2.fq.gz -S s141.bt2.sam --no-unal --al ./s141.al --un symbionts/s141.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s141_R1_001_val_1.fq.gz -2 s141_R2_001_val_2.fq.gz -S s141.bt2.sam --no-unal --al-conc ./s141.al --un-conc symbionts/s141.un</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -9226,7 +9226,7 @@
       </c>
       <c r="H142" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s142_R1_001_val_1.fq.gz -2 s142_R2_001_val_2.fq.gz -S s142.bt2.sam --no-unal --al ./s142.al --un symbionts/s142.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s142_R1_001_val_1.fq.gz -2 s142_R2_001_val_2.fq.gz -S s142.bt2.sam --no-unal --al-conc ./s142.al --un-conc symbionts/s142.un</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -9241,7 +9241,7 @@
       </c>
       <c r="H143" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s143_R1_001_val_1.fq.gz -2 s143_R2_001_val_2.fq.gz -S s143.bt2.sam --no-unal --al ./s143.al --un symbionts/s143.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s143_R1_001_val_1.fq.gz -2 s143_R2_001_val_2.fq.gz -S s143.bt2.sam --no-unal --al-conc ./s143.al --un-conc symbionts/s143.un</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -9256,7 +9256,7 @@
       </c>
       <c r="H144" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s144_R1_001_val_1.fq.gz -2 s144_R2_001_val_2.fq.gz -S s144.bt2.sam --no-unal --al ./s144.al --un symbionts/s144.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s144_R1_001_val_1.fq.gz -2 s144_R2_001_val_2.fq.gz -S s144.bt2.sam --no-unal --al-conc ./s144.al --un-conc symbionts/s144.un</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -9271,7 +9271,7 @@
       </c>
       <c r="H145" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s145_R1_001_val_1.fq.gz -2 s145_R2_001_val_2.fq.gz -S s145.bt2.sam --no-unal --al ./s145.al --un symbionts/s145.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s145_R1_001_val_1.fq.gz -2 s145_R2_001_val_2.fq.gz -S s145.bt2.sam --no-unal --al-conc ./s145.al --un-conc symbionts/s145.un</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -9286,7 +9286,7 @@
       </c>
       <c r="H146" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s146_R1_001_val_1.fq.gz -2 s146_R2_001_val_2.fq.gz -S s146.bt2.sam --no-unal --al ./s146.al --un symbionts/s146.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s146_R1_001_val_1.fq.gz -2 s146_R2_001_val_2.fq.gz -S s146.bt2.sam --no-unal --al-conc ./s146.al --un-conc symbionts/s146.un</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -9301,7 +9301,7 @@
       </c>
       <c r="H147" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s147_R1_001_val_1.fq.gz -2 s147_R2_001_val_2.fq.gz -S s147.bt2.sam --no-unal --al ./s147.al --un symbionts/s147.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s147_R1_001_val_1.fq.gz -2 s147_R2_001_val_2.fq.gz -S s147.bt2.sam --no-unal --al-conc ./s147.al --un-conc symbionts/s147.un</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -9316,7 +9316,7 @@
       </c>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s148_R1_001_val_1.fq.gz -2 s148_R2_001_val_2.fq.gz -S s148.bt2.sam --no-unal --al ./s148.al --un symbionts/s148.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s148_R1_001_val_1.fq.gz -2 s148_R2_001_val_2.fq.gz -S s148.bt2.sam --no-unal --al-conc ./s148.al --un-conc symbionts/s148.un</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -9331,7 +9331,7 @@
       </c>
       <c r="H149" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s149_R1_001_val_1.fq.gz -2 s149_R2_001_val_2.fq.gz -S s149.bt2.sam --no-unal --al ./s149.al --un symbionts/s149.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s149_R1_001_val_1.fq.gz -2 s149_R2_001_val_2.fq.gz -S s149.bt2.sam --no-unal --al-conc ./s149.al --un-conc symbionts/s149.un</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -9346,7 +9346,7 @@
       </c>
       <c r="H150" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s150_R1_001_val_1.fq.gz -2 s150_R2_001_val_2.fq.gz -S s150.bt2.sam --no-unal --al ./s150.al --un symbionts/s150.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s150_R1_001_val_1.fq.gz -2 s150_R2_001_val_2.fq.gz -S s150.bt2.sam --no-unal --al-conc ./s150.al --un-conc symbionts/s150.un</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="H151" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s151_R1_001_val_1.fq.gz -2 s151_R2_001_val_2.fq.gz -S s151.bt2.sam --no-unal --al ./s151.al --un symbionts/s151.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s151_R1_001_val_1.fq.gz -2 s151_R2_001_val_2.fq.gz -S s151.bt2.sam --no-unal --al-conc ./s151.al --un-conc symbionts/s151.un</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -9376,7 +9376,7 @@
       </c>
       <c r="H152" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s152_R1_001_val_1.fq.gz -2 s152_R2_001_val_2.fq.gz -S s152.bt2.sam --no-unal --al ./s152.al --un symbionts/s152.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s152_R1_001_val_1.fq.gz -2 s152_R2_001_val_2.fq.gz -S s152.bt2.sam --no-unal --al-conc ./s152.al --un-conc symbionts/s152.un</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="H153" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s153_R1_001_val_1.fq.gz -2 s153_R2_001_val_2.fq.gz -S s153.bt2.sam --no-unal --al ./s153.al --un symbionts/s153.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s153_R1_001_val_1.fq.gz -2 s153_R2_001_val_2.fq.gz -S s153.bt2.sam --no-unal --al-conc ./s153.al --un-conc symbionts/s153.un</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -9406,7 +9406,7 @@
       </c>
       <c r="H154" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s154_R1_001_val_1.fq.gz -2 s154_R2_001_val_2.fq.gz -S s154.bt2.sam --no-unal --al ./s154.al --un symbionts/s154.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s154_R1_001_val_1.fq.gz -2 s154_R2_001_val_2.fq.gz -S s154.bt2.sam --no-unal --al-conc ./s154.al --un-conc symbionts/s154.un</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -9421,7 +9421,7 @@
       </c>
       <c r="H155" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s155_R1_001_val_1.fq.gz -2 s155_R2_001_val_2.fq.gz -S s155.bt2.sam --no-unal --al ./s155.al --un symbionts/s155.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s155_R1_001_val_1.fq.gz -2 s155_R2_001_val_2.fq.gz -S s155.bt2.sam --no-unal --al-conc ./s155.al --un-conc symbionts/s155.un</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="H156" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s156_R1_001_val_1.fq.gz -2 s156_R2_001_val_2.fq.gz -S s156.bt2.sam --no-unal --al ./s156.al --un symbionts/s156.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s156_R1_001_val_1.fq.gz -2 s156_R2_001_val_2.fq.gz -S s156.bt2.sam --no-unal --al-conc ./s156.al --un-conc symbionts/s156.un</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -9451,7 +9451,7 @@
       </c>
       <c r="H157" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s157_R1_001_val_1.fq.gz -2 s157_R2_001_val_2.fq.gz -S s157.bt2.sam --no-unal --al ./s157.al --un symbionts/s157.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s157_R1_001_val_1.fq.gz -2 s157_R2_001_val_2.fq.gz -S s157.bt2.sam --no-unal --al-conc ./s157.al --un-conc symbionts/s157.un</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -9466,7 +9466,7 @@
       </c>
       <c r="H158" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s158_R1_001_val_1.fq.gz -2 s158_R2_001_val_2.fq.gz -S s158.bt2.sam --no-unal --al ./s158.al --un symbionts/s158.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s158_R1_001_val_1.fq.gz -2 s158_R2_001_val_2.fq.gz -S s158.bt2.sam --no-unal --al-conc ./s158.al --un-conc symbionts/s158.un</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -9481,7 +9481,7 @@
       </c>
       <c r="H159" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s159_R1_001_val_1.fq.gz -2 s159_R2_001_val_2.fq.gz -S s159.bt2.sam --no-unal --al ./s159.al --un symbionts/s159.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s159_R1_001_val_1.fq.gz -2 s159_R2_001_val_2.fq.gz -S s159.bt2.sam --no-unal --al-conc ./s159.al --un-conc symbionts/s159.un</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -9496,7 +9496,7 @@
       </c>
       <c r="H160" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s160_R1_001_val_1.fq.gz -2 s160_R2_001_val_2.fq.gz -S s160.bt2.sam --no-unal --al ./s160.al --un symbionts/s160.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s160_R1_001_val_1.fq.gz -2 s160_R2_001_val_2.fq.gz -S s160.bt2.sam --no-unal --al-conc ./s160.al --un-conc symbionts/s160.un</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -9511,7 +9511,7 @@
       </c>
       <c r="H161" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s161_R1_001_val_1.fq.gz -2 s161_R2_001_val_2.fq.gz -S s161.bt2.sam --no-unal --al ./s161.al --un symbionts/s161.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s161_R1_001_val_1.fq.gz -2 s161_R2_001_val_2.fq.gz -S s161.bt2.sam --no-unal --al-conc ./s161.al --un-conc symbionts/s161.un</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
@@ -9526,7 +9526,7 @@
       </c>
       <c r="H162" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s162_R1_001_val_1.fq.gz -2 s162_R2_001_val_2.fq.gz -S s162.bt2.sam --no-unal --al ./s162.al --un symbionts/s162.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s162_R1_001_val_1.fq.gz -2 s162_R2_001_val_2.fq.gz -S s162.bt2.sam --no-unal --al-conc ./s162.al --un-conc symbionts/s162.un</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -9541,7 +9541,7 @@
       </c>
       <c r="H163" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s163_R1_001_val_1.fq.gz -2 s163_R2_001_val_2.fq.gz -S s163.bt2.sam --no-unal --al ./s163.al --un symbionts/s163.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s163_R1_001_val_1.fq.gz -2 s163_R2_001_val_2.fq.gz -S s163.bt2.sam --no-unal --al-conc ./s163.al --un-conc symbionts/s163.un</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -9556,7 +9556,7 @@
       </c>
       <c r="H164" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s164_R1_001_val_1.fq.gz -2 s164_R2_001_val_2.fq.gz -S s164.bt2.sam --no-unal --al ./s164.al --un symbionts/s164.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s164_R1_001_val_1.fq.gz -2 s164_R2_001_val_2.fq.gz -S s164.bt2.sam --no-unal --al-conc ./s164.al --un-conc symbionts/s164.un</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -9571,7 +9571,7 @@
       </c>
       <c r="H165" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s165_R1_001_val_1.fq.gz -2 s165_R2_001_val_2.fq.gz -S s165.bt2.sam --no-unal --al ./s165.al --un symbionts/s165.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s165_R1_001_val_1.fq.gz -2 s165_R2_001_val_2.fq.gz -S s165.bt2.sam --no-unal --al-conc ./s165.al --un-conc symbionts/s165.un</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="H166" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s166_R1_001_val_1.fq.gz -2 s166_R2_001_val_2.fq.gz -S s166.bt2.sam --no-unal --al ./s166.al --un symbionts/s166.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s166_R1_001_val_1.fq.gz -2 s166_R2_001_val_2.fq.gz -S s166.bt2.sam --no-unal --al-conc ./s166.al --un-conc symbionts/s166.un</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="H167" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s167_R1_001_val_1.fq.gz -2 s167_R2_001_val_2.fq.gz -S s167.bt2.sam --no-unal --al ./s167.al --un symbionts/s167.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s167_R1_001_val_1.fq.gz -2 s167_R2_001_val_2.fq.gz -S s167.bt2.sam --no-unal --al-conc ./s167.al --un-conc symbionts/s167.un</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -9616,7 +9616,7 @@
       </c>
       <c r="H168" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s168_R1_001_val_1.fq.gz -2 s168_R2_001_val_2.fq.gz -S s168.bt2.sam --no-unal --al ./s168.al --un symbionts/s168.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s168_R1_001_val_1.fq.gz -2 s168_R2_001_val_2.fq.gz -S s168.bt2.sam --no-unal --al-conc ./s168.al --un-conc symbionts/s168.un</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -9631,7 +9631,7 @@
       </c>
       <c r="H169" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s169_R1_001_val_1.fq.gz -2 s169_R2_001_val_2.fq.gz -S s169.bt2.sam --no-unal --al ./s169.al --un symbionts/s169.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s169_R1_001_val_1.fq.gz -2 s169_R2_001_val_2.fq.gz -S s169.bt2.sam --no-unal --al-conc ./s169.al --un-conc symbionts/s169.un</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -9646,7 +9646,7 @@
       </c>
       <c r="H170" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s170_R1_001_val_1.fq.gz -2 s170_R2_001_val_2.fq.gz -S s170.bt2.sam --no-unal --al ./s170.al --un symbionts/s170.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s170_R1_001_val_1.fq.gz -2 s170_R2_001_val_2.fq.gz -S s170.bt2.sam --no-unal --al-conc ./s170.al --un-conc symbionts/s170.un</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="H171" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s171_R1_001_val_1.fq.gz -2 s171_R2_001_val_2.fq.gz -S s171.bt2.sam --no-unal --al ./s171.al --un symbionts/s171.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s171_R1_001_val_1.fq.gz -2 s171_R2_001_val_2.fq.gz -S s171.bt2.sam --no-unal --al-conc ./s171.al --un-conc symbionts/s171.un</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -9676,7 +9676,7 @@
       </c>
       <c r="H172" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s172_R1_001_val_1.fq.gz -2 s172_R2_001_val_2.fq.gz -S s172.bt2.sam --no-unal --al ./s172.al --un symbionts/s172.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s172_R1_001_val_1.fq.gz -2 s172_R2_001_val_2.fq.gz -S s172.bt2.sam --no-unal --al-conc ./s172.al --un-conc symbionts/s172.un</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="H173" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s173_R1_001_val_1.fq.gz -2 s173_R2_001_val_2.fq.gz -S s173.bt2.sam --no-unal --al ./s173.al --un symbionts/s173.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s173_R1_001_val_1.fq.gz -2 s173_R2_001_val_2.fq.gz -S s173.bt2.sam --no-unal --al-conc ./s173.al --un-conc symbionts/s173.un</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -9706,7 +9706,7 @@
       </c>
       <c r="H174" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s174_R1_001_val_1.fq.gz -2 s174_R2_001_val_2.fq.gz -S s174.bt2.sam --no-unal --al ./s174.al --un symbionts/s174.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s174_R1_001_val_1.fq.gz -2 s174_R2_001_val_2.fq.gz -S s174.bt2.sam --no-unal --al-conc ./s174.al --un-conc symbionts/s174.un</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="H175" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s175_R1_001_val_1.fq.gz -2 s175_R2_001_val_2.fq.gz -S s175.bt2.sam --no-unal --al ./s175.al --un symbionts/s175.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s175_R1_001_val_1.fq.gz -2 s175_R2_001_val_2.fq.gz -S s175.bt2.sam --no-unal --al-conc ./s175.al --un-conc symbionts/s175.un</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -9736,7 +9736,7 @@
       </c>
       <c r="H176" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s176_R1_001_val_1.fq.gz -2 s176_R2_001_val_2.fq.gz -S s176.bt2.sam --no-unal --al ./s176.al --un symbionts/s176.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s176_R1_001_val_1.fq.gz -2 s176_R2_001_val_2.fq.gz -S s176.bt2.sam --no-unal --al-conc ./s176.al --un-conc symbionts/s176.un</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -9751,7 +9751,7 @@
       </c>
       <c r="H177" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s177_R1_001_val_1.fq.gz -2 s177_R2_001_val_2.fq.gz -S s177.bt2.sam --no-unal --al ./s177.al --un symbionts/s177.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s177_R1_001_val_1.fq.gz -2 s177_R2_001_val_2.fq.gz -S s177.bt2.sam --no-unal --al-conc ./s177.al --un-conc symbionts/s177.un</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -9766,7 +9766,7 @@
       </c>
       <c r="H178" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s178_R1_001_val_1.fq.gz -2 s178_R2_001_val_2.fq.gz -S s178.bt2.sam --no-unal --al ./s178.al --un symbionts/s178.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s178_R1_001_val_1.fq.gz -2 s178_R2_001_val_2.fq.gz -S s178.bt2.sam --no-unal --al-conc ./s178.al --un-conc symbionts/s178.un</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -9781,7 +9781,7 @@
       </c>
       <c r="H179" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s179_R1_001_val_1.fq.gz -2 s179_R2_001_val_2.fq.gz -S s179.bt2.sam --no-unal --al ./s179.al --un symbionts/s179.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s179_R1_001_val_1.fq.gz -2 s179_R2_001_val_2.fq.gz -S s179.bt2.sam --no-unal --al-conc ./s179.al --un-conc symbionts/s179.un</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -9796,7 +9796,7 @@
       </c>
       <c r="H180" t="str">
         <f t="shared" si="2"/>
-        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s180_R1_001_val_1.fq.gz -2 s180_R2_001_val_2.fq.gz -S s180.bt2.sam --no-unal --al ./s180.al --un symbionts/s180.un</v>
+        <v>bowtie2 --score-min L,16,1 --local -L 16 -p 2 -x /mnt/beegfs/home/mstudiva/db/ofavgenome/OfaveolataGenome -1 s180_R1_001_val_1.fq.gz -2 s180_R2_001_val_2.fq.gz -S s180.bt2.sam --no-unal --al-conc ./s180.al --un-conc symbionts/s180.un</v>
       </c>
     </row>
   </sheetData>

</xml_diff>